<commit_message>
estoy cambiando de lap
</commit_message>
<xml_diff>
--- a/seeders/docentes_cursos.xlsx
+++ b/seeders/docentes_cursos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos_Nick\Python\notas_jhon\backendSistNotas\seeders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloyd\Desktop\sistema notas\backendSistNotas\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9237FF-4BB2-4AE2-9E54-BC66FDB81226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F8AC9F-9B52-423F-83EF-44D413D3BF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{3B7EAE99-D4F4-4E5C-9D99-0542953DEDE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{3B7EAE99-D4F4-4E5C-9D99-0542953DEDE9}"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -445,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -475,28 +472,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -504,8 +486,11 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -539,11 +524,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -821,10 +803,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89632221-E480-454C-A8C7-75F3FD8D1543}" name="Tabla2" displayName="Tabla2" ref="A1:E44" totalsRowShown="0" tableBorderDxfId="4">
   <autoFilter ref="A1:E44" xr:uid="{89632221-E480-454C-A8C7-75F3FD8D1543}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{3D5A8A4E-4D0D-4582-9952-72E577976709}" name="N°" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{88638D52-5F9D-45F5-B31A-5D0F8E40A5A7}" name="cursos" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{60D0C51E-FEB2-49EF-BF4E-2F393BBEE523}" name="ciclos" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{BC90EDA6-ADC0-43A5-849C-5974931AAB0E}" name="Docente" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3D5A8A4E-4D0D-4582-9952-72E577976709}" name="N°" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{88638D52-5F9D-45F5-B31A-5D0F8E40A5A7}" name="cursos" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{60D0C51E-FEB2-49EF-BF4E-2F393BBEE523}" name="ciclos" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{BC90EDA6-ADC0-43A5-849C-5974931AAB0E}" name="Docente" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{CA10EE53-EF5E-43A9-BD11-E3A7A0F5AFFB}" name="año"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1131,7 +1113,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="134" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1164,7 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="13">
         <v>35245618</v>
       </c>
       <c r="C2" t="s">
@@ -1209,7 +1191,7 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="12">
         <v>41493216</v>
       </c>
       <c r="C3" t="s">
@@ -1236,7 +1218,7 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="12">
         <v>46504162</v>
       </c>
       <c r="C4" t="s">
@@ -1263,7 +1245,7 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="12">
         <v>46275055</v>
       </c>
       <c r="C5" t="s">
@@ -1290,7 +1272,7 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="12">
         <v>72107732</v>
       </c>
       <c r="C6" t="s">
@@ -1317,10 +1299,10 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="14">
         <v>45448795</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" t="s">
         <v>83</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -1354,7 +1336,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1347,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -1382,22 +1364,22 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="12">
         <v>41493216</v>
       </c>
       <c r="E2">
         <v>2025</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <v>35245618</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -1405,16 +1387,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="13">
         <v>35245618</v>
       </c>
       <c r="E3">
@@ -1428,16 +1410,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <v>72107732</v>
       </c>
       <c r="E4">
@@ -1451,16 +1433,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="12">
         <v>46504162</v>
       </c>
       <c r="E5">
@@ -1474,16 +1456,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <v>41493216</v>
       </c>
       <c r="E6">
@@ -1497,39 +1479,39 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="13">
         <v>35245618</v>
       </c>
       <c r="E7">
         <v>2025</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="2">
         <v>45448795</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="12">
         <v>46275055</v>
       </c>
       <c r="E8">
@@ -1537,16 +1519,16 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="12">
         <v>72107732</v>
       </c>
       <c r="E9">
@@ -1554,16 +1536,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="12">
         <v>41493216</v>
       </c>
       <c r="E10">
@@ -1571,16 +1553,16 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="12">
         <v>46504162</v>
       </c>
       <c r="E11">
@@ -1588,16 +1570,16 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="16">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="13">
         <v>35245618</v>
       </c>
       <c r="E12">
@@ -1605,16 +1587,16 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="12">
         <v>46504162</v>
       </c>
       <c r="E13">
@@ -1622,16 +1604,16 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <v>72107732</v>
       </c>
       <c r="E14">
@@ -1639,16 +1621,16 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="12">
         <v>41493216</v>
       </c>
       <c r="E15">
@@ -1656,16 +1638,16 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="12">
         <v>46275055</v>
       </c>
       <c r="E16">
@@ -1673,16 +1655,16 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="12">
         <v>46275055</v>
       </c>
       <c r="E17">
@@ -1690,16 +1672,16 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
+      <c r="A18" s="16">
         <v>17</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="12">
         <v>72107732</v>
       </c>
       <c r="E18">
@@ -1707,16 +1689,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
+      <c r="A19" s="16">
         <v>18</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="12">
         <v>46504162</v>
       </c>
       <c r="E19">
@@ -1724,16 +1706,16 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="15">
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="12">
         <v>41493216</v>
       </c>
       <c r="E20">
@@ -1741,16 +1723,16 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
+      <c r="A21" s="16">
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="12">
         <v>45448795</v>
       </c>
       <c r="E21">
@@ -1758,16 +1740,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="23">
+      <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="13">
         <v>35245618</v>
       </c>
       <c r="E22">
@@ -1775,16 +1757,16 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="15">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="12">
         <v>46275055</v>
       </c>
       <c r="E23">
@@ -1792,16 +1774,16 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="23">
+      <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="12">
         <v>72107732</v>
       </c>
       <c r="E24">
@@ -1809,16 +1791,16 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
+      <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="13">
         <v>35245618</v>
       </c>
       <c r="E25">
@@ -1826,16 +1808,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
+      <c r="A26" s="15">
         <v>25</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="12">
         <v>41493216</v>
       </c>
       <c r="E26">
@@ -1843,16 +1825,16 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
+      <c r="A27" s="16">
         <v>26</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="12">
         <v>46275055</v>
       </c>
       <c r="E27">
@@ -1860,16 +1842,16 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="16">
         <v>27</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="12">
         <v>45448795</v>
       </c>
       <c r="E28">
@@ -1877,16 +1859,16 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="21">
+      <c r="A29" s="15">
         <v>28</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="12">
         <v>72107732</v>
       </c>
       <c r="E29">
@@ -1894,16 +1876,16 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="23">
+      <c r="A30" s="16">
         <v>29</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="12">
         <v>72107732</v>
       </c>
       <c r="E30">
@@ -1911,16 +1893,16 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="23">
+      <c r="A31" s="16">
         <v>30</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="12">
         <v>46504162</v>
       </c>
       <c r="E31">
@@ -1928,16 +1910,16 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
+      <c r="A32" s="15">
         <v>31</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="12">
         <v>46504162</v>
       </c>
       <c r="E32">
@@ -1945,16 +1927,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="23">
+      <c r="A33" s="16">
         <v>32</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="12">
         <v>46275055</v>
       </c>
       <c r="E33">
@@ -1962,16 +1944,16 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="23">
+      <c r="A34" s="16">
         <v>33</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="12">
         <v>46275055</v>
       </c>
       <c r="E34">
@@ -1979,16 +1961,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="21">
+      <c r="A35" s="15">
         <v>34</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="13">
         <v>35245618</v>
       </c>
       <c r="E35">
@@ -1996,16 +1978,16 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="23">
+      <c r="A36" s="16">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="12">
         <v>72107732</v>
       </c>
       <c r="E36">
@@ -2013,16 +1995,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="23">
+      <c r="A37" s="16">
         <v>36</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="12">
         <v>41493216</v>
       </c>
       <c r="E37">
@@ -2030,16 +2012,16 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="21">
+      <c r="A38" s="15">
         <v>37</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="12">
         <v>46504162</v>
       </c>
       <c r="E38">
@@ -2047,16 +2029,16 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
+      <c r="A39" s="16">
         <v>38</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="12">
         <v>46275055</v>
       </c>
       <c r="E39">
@@ -2064,16 +2046,16 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="23">
+      <c r="A40" s="16">
         <v>39</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="12">
         <v>72107732</v>
       </c>
       <c r="E40">
@@ -2081,16 +2063,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="21">
+      <c r="A41" s="15">
         <v>40</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D41" s="12">
         <v>72107732</v>
       </c>
       <c r="E41">
@@ -2098,16 +2080,16 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="23">
+      <c r="A42" s="16">
         <v>41</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D42" s="12">
         <v>46275055</v>
       </c>
       <c r="E42">
@@ -2115,16 +2097,16 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="23">
+      <c r="A43" s="16">
         <v>42</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="19">
+      <c r="D43" s="13">
         <v>35245618</v>
       </c>
       <c r="E43">
@@ -2132,16 +2114,16 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="21">
+      <c r="A44" s="15">
         <v>43</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="16">
+      <c r="D44" s="12">
         <v>41493216</v>
       </c>
       <c r="E44">

</xml_diff>